<commit_message>
added zspread calculation module. Split out progress bar into a separate module and added functionality. Improved spot curve interpolation
</commit_message>
<xml_diff>
--- a/GBP Bonds/Master List of Bonds/Consumer Goods.xlsx
+++ b/GBP Bonds/Master List of Bonds/Consumer Goods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renea\OneDrive\Documents\University of Bath\13. Dissertation\Data\GBP Bonds\Master List of Bonds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C1FC6-2FBA-4BFD-85A7-0317363C92E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C864A60-5521-48EF-BEC0-9F2FAC25BB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="134">
   <si>
     <t>Issuer</t>
   </si>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1126,9 +1126,7 @@
       <c r="AT2" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" t="s">
-        <v>19</v>
-      </c>
+      <c r="AU2" s="2"/>
       <c r="AV2" t="s">
         <v>19</v>
       </c>
@@ -3624,8 +3622,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AZ1 A15:AZ18 A2:F2 H2:AZ2 A3:F3 H3:AZ3 A4:F4 H4:AZ4 A5:F5 H5:AZ5 A6:F6 H6:AZ6 A7:F7 H7:AZ7 A8:F8 H8:AZ8 A9:F9 H9:AZ9 A10:F10 H10:AZ10 A11:F11 H11:AZ11 A12:F12 H12:AZ12 A13:F13 H13:AZ13 A14:F14 H14:AZ14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AZ1 A15:AZ18 A2:F2 H2:AT2 A3:F3 H3:AZ3 A4:F4 H4:AZ4 A5:F5 H5:AZ5 A6:F6 H6:AZ6 A7:F7 H7:AZ7 A8:F8 H8:AZ8 A9:F9 H9:AZ9 A10:F10 H10:AZ10 A11:F11 H11:AZ11 A12:F12 H12:AZ12 A13:F13 H13:AZ13 A14:F14 H14:AZ14 AV2:AZ2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>